<commit_message>
bf: update some forms
</commit_message>
<xml_diff>
--- a/LF/TAS/Burkina Faso/2023/september/bf_lf_tas1_202309_3_resultats_fts.xlsx
+++ b/LF/TAS/Burkina Faso/2023/september/bf_lf_tas1_202309_3_resultats_fts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\yumbad\Repositories\dsa-forms\LF\TAS\Burkina Faso\2023\september\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63385F7C-36F7-473E-A348-6A6C4575932F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{83C6860B-C385-4896-9300-DF62ABEDF84C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1380" yWindow="3405" windowWidth="28800" windowHeight="15435" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1289" uniqueCount="514">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1289" uniqueCount="512">
   <si>
     <t>type</t>
   </si>
@@ -1277,12 +1277,6 @@
     <t>d_numero_ordre_grappe</t>
   </si>
   <si>
-    <t>CENTRE EST</t>
-  </si>
-  <si>
-    <t>SUD OUEST</t>
-  </si>
-  <si>
     <t>DIMISTENGA</t>
   </si>
   <si>
@@ -1550,12 +1544,6 @@
     <t>N.TONHERO</t>
   </si>
   <si>
-    <t>(Sept 2023) Burkina Faso TAS FL - 3. Formulaire Résultat FTS V2</t>
-  </si>
-  <si>
-    <t>bf_lf_tas1_202309_3_resultats_fts_v2</t>
-  </si>
-  <si>
     <t>006 (LIOULGOU)</t>
   </si>
   <si>
@@ -1755,6 +1743,12 @@
   </si>
   <si>
     <t>017 (OBRO)</t>
+  </si>
+  <si>
+    <t>(Sept 2023) Burkina Faso TAS FL - 3. Formulaire Résultat FTS V2.1</t>
+  </si>
+  <si>
+    <t>bf_lf_tas1_202309_3_resultats_fts_v2_1</t>
   </si>
 </sst>
 </file>
@@ -2270,7 +2264,7 @@
       <pane xSplit="3" ySplit="1" topLeftCell="D2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C27" sqref="C27"/>
+      <selection pane="bottomRight" activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3281,8 +3275,8 @@
   <dimension ref="A1:H280"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A54" sqref="A54:XFD280"/>
+      <pane ySplit="1" topLeftCell="A26" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A44" sqref="A44:XFD280"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -3737,13 +3731,13 @@
         <v>182</v>
       </c>
       <c r="B47" t="s">
-        <v>354</v>
+        <v>241</v>
       </c>
       <c r="C47" t="s">
-        <v>354</v>
+        <v>241</v>
       </c>
       <c r="D47" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="48" spans="1:4">
@@ -3751,13 +3745,13 @@
         <v>182</v>
       </c>
       <c r="B48" t="s">
-        <v>355</v>
+        <v>242</v>
       </c>
       <c r="C48" t="s">
-        <v>355</v>
+        <v>242</v>
       </c>
       <c r="D48" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
     </row>
     <row r="50" spans="1:5">
@@ -4260,10 +4254,10 @@
         <v>184</v>
       </c>
       <c r="B88" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="C88" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="F88" t="s">
         <v>250</v>
@@ -4428,10 +4422,10 @@
         <v>184</v>
       </c>
       <c r="B100" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="C100" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="F100" t="s">
         <v>251</v>
@@ -4540,10 +4534,10 @@
         <v>184</v>
       </c>
       <c r="B108" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="C108" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="F108" t="s">
         <v>253</v>
@@ -4792,10 +4786,10 @@
         <v>185</v>
       </c>
       <c r="B127" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C127" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="G127" t="s">
         <v>261</v>
@@ -4834,10 +4828,10 @@
         <v>185</v>
       </c>
       <c r="B130" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="C130" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="G130" t="s">
         <v>261</v>
@@ -4910,7 +4904,7 @@
         <v>279</v>
       </c>
       <c r="G135" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
     </row>
     <row r="136" spans="1:7">
@@ -5100,10 +5094,10 @@
         <v>185</v>
       </c>
       <c r="B149" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="C149" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="G149" t="s">
         <v>242</v>
@@ -5114,10 +5108,10 @@
         <v>185</v>
       </c>
       <c r="B150" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="C150" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="G150" t="s">
         <v>242</v>
@@ -5128,10 +5122,10 @@
         <v>185</v>
       </c>
       <c r="B151" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="C151" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="G151" t="s">
         <v>242</v>
@@ -5156,10 +5150,10 @@
         <v>185</v>
       </c>
       <c r="B153" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C153" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="G153" t="s">
         <v>242</v>
@@ -5170,10 +5164,10 @@
         <v>185</v>
       </c>
       <c r="B154" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="C154" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="G154" t="s">
         <v>242</v>
@@ -5184,10 +5178,10 @@
         <v>185</v>
       </c>
       <c r="B155" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C155" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="G155" t="s">
         <v>242</v>
@@ -5198,10 +5192,10 @@
         <v>185</v>
       </c>
       <c r="B156" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C156" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="G156" t="s">
         <v>242</v>
@@ -5212,10 +5206,10 @@
         <v>185</v>
       </c>
       <c r="B157" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="C157" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="G157" t="s">
         <v>242</v>
@@ -5358,7 +5352,7 @@
         <v>285</v>
       </c>
       <c r="G167" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
     </row>
     <row r="168" spans="1:7">
@@ -5386,7 +5380,7 @@
         <v>338</v>
       </c>
       <c r="G169" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
     </row>
     <row r="170" spans="1:7">
@@ -5394,7 +5388,7 @@
         <v>185</v>
       </c>
       <c r="B170" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
       <c r="C170" t="s">
         <v>308</v>
@@ -5758,10 +5752,10 @@
         <v>235</v>
       </c>
       <c r="B197" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="C197" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="H197" t="s">
         <v>272</v>
@@ -5772,10 +5766,10 @@
         <v>235</v>
       </c>
       <c r="B198" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="C198" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="H198" t="s">
         <v>273</v>
@@ -5786,10 +5780,10 @@
         <v>235</v>
       </c>
       <c r="B199" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="C199" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="H199" t="s">
         <v>318</v>
@@ -5800,10 +5794,10 @@
         <v>235</v>
       </c>
       <c r="B200" t="s">
-        <v>448</v>
+        <v>444</v>
       </c>
       <c r="C200" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="H200" t="s">
         <v>319</v>
@@ -5814,10 +5808,10 @@
         <v>235</v>
       </c>
       <c r="B201" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="C201" t="s">
-        <v>376</v>
+        <v>374</v>
       </c>
       <c r="H201" t="s">
         <v>249</v>
@@ -5828,10 +5822,10 @@
         <v>235</v>
       </c>
       <c r="B202" t="s">
-        <v>449</v>
+        <v>445</v>
       </c>
       <c r="C202" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="H202" t="s">
         <v>317</v>
@@ -5842,10 +5836,10 @@
         <v>235</v>
       </c>
       <c r="B203" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C203" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="H203" t="s">
         <v>278</v>
@@ -5856,10 +5850,10 @@
         <v>235</v>
       </c>
       <c r="B204" t="s">
-        <v>450</v>
+        <v>446</v>
       </c>
       <c r="C204" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="H204" t="s">
         <v>320</v>
@@ -5870,10 +5864,10 @@
         <v>235</v>
       </c>
       <c r="B205" t="s">
-        <v>451</v>
+        <v>447</v>
       </c>
       <c r="C205" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="H205" t="s">
         <v>316</v>
@@ -5884,10 +5878,10 @@
         <v>235</v>
       </c>
       <c r="B206" t="s">
-        <v>452</v>
+        <v>448</v>
       </c>
       <c r="C206" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="H206" t="s">
         <v>325</v>
@@ -5898,10 +5892,10 @@
         <v>235</v>
       </c>
       <c r="B207" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="C207" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="H207" t="s">
         <v>279</v>
@@ -5912,10 +5906,10 @@
         <v>235</v>
       </c>
       <c r="B208" t="s">
-        <v>454</v>
+        <v>450</v>
       </c>
       <c r="C208" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="H208" t="s">
         <v>324</v>
@@ -5926,10 +5920,10 @@
         <v>235</v>
       </c>
       <c r="B209" t="s">
-        <v>455</v>
+        <v>451</v>
       </c>
       <c r="C209" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="H209" t="s">
         <v>323</v>
@@ -5940,10 +5934,10 @@
         <v>235</v>
       </c>
       <c r="B210" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="C210" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="H210" t="s">
         <v>276</v>
@@ -5954,10 +5948,10 @@
         <v>235</v>
       </c>
       <c r="B211" t="s">
-        <v>456</v>
+        <v>452</v>
       </c>
       <c r="C211" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="H211" t="s">
         <v>322</v>
@@ -5968,10 +5962,10 @@
         <v>235</v>
       </c>
       <c r="B212" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
       <c r="C212" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="H212" t="s">
         <v>333</v>
@@ -5982,10 +5976,10 @@
         <v>235</v>
       </c>
       <c r="B213" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
       <c r="C213" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="H213" t="s">
         <v>332</v>
@@ -5996,10 +5990,10 @@
         <v>235</v>
       </c>
       <c r="B214" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="C214" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="H214" t="s">
         <v>335</v>
@@ -6010,10 +6004,10 @@
         <v>235</v>
       </c>
       <c r="B215" t="s">
-        <v>460</v>
+        <v>456</v>
       </c>
       <c r="C215" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="H215" t="s">
         <v>336</v>
@@ -6024,10 +6018,10 @@
         <v>235</v>
       </c>
       <c r="B216" t="s">
-        <v>461</v>
+        <v>457</v>
       </c>
       <c r="C216" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="H216" t="s">
         <v>339</v>
@@ -6038,10 +6032,10 @@
         <v>235</v>
       </c>
       <c r="B217" t="s">
-        <v>462</v>
+        <v>458</v>
       </c>
       <c r="C217" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="H217" t="s">
         <v>340</v>
@@ -6052,10 +6046,10 @@
         <v>235</v>
       </c>
       <c r="B218" t="s">
-        <v>463</v>
+        <v>459</v>
       </c>
       <c r="C218" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="H218" t="s">
         <v>338</v>
@@ -6066,10 +6060,10 @@
         <v>235</v>
       </c>
       <c r="B219" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="C219" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="H219" t="s">
         <v>275</v>
@@ -6080,10 +6074,10 @@
         <v>235</v>
       </c>
       <c r="B220" t="s">
-        <v>464</v>
+        <v>460</v>
       </c>
       <c r="C220" t="s">
-        <v>374</v>
+        <v>372</v>
       </c>
       <c r="H220" t="s">
         <v>327</v>
@@ -6094,10 +6088,10 @@
         <v>235</v>
       </c>
       <c r="B221" t="s">
-        <v>396</v>
+        <v>394</v>
       </c>
       <c r="C221" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="H221" t="s">
         <v>286</v>
@@ -6108,10 +6102,10 @@
         <v>235</v>
       </c>
       <c r="B222" t="s">
-        <v>465</v>
+        <v>461</v>
       </c>
       <c r="C222" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="H222" t="s">
         <v>285</v>
@@ -6122,10 +6116,10 @@
         <v>235</v>
       </c>
       <c r="B223" t="s">
-        <v>398</v>
+        <v>396</v>
       </c>
       <c r="C223" t="s">
-        <v>399</v>
+        <v>397</v>
       </c>
       <c r="H223" t="s">
         <v>284</v>
@@ -6136,13 +6130,13 @@
         <v>235</v>
       </c>
       <c r="B224" t="s">
-        <v>466</v>
+        <v>462</v>
       </c>
       <c r="C224" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="H224" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
     </row>
     <row r="225" spans="1:8">
@@ -6150,13 +6144,13 @@
         <v>235</v>
       </c>
       <c r="B225" t="s">
-        <v>467</v>
+        <v>463</v>
       </c>
       <c r="C225" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="H225" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
     </row>
     <row r="226" spans="1:8">
@@ -6164,13 +6158,13 @@
         <v>235</v>
       </c>
       <c r="B226" t="s">
-        <v>468</v>
+        <v>464</v>
       </c>
       <c r="C226" t="s">
-        <v>400</v>
+        <v>398</v>
       </c>
       <c r="H226" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
     </row>
     <row r="227" spans="1:8">
@@ -6178,13 +6172,13 @@
         <v>235</v>
       </c>
       <c r="B227" t="s">
-        <v>469</v>
+        <v>465</v>
       </c>
       <c r="C227" t="s">
-        <v>401</v>
+        <v>399</v>
       </c>
       <c r="H227" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
     </row>
     <row r="228" spans="1:8">
@@ -6192,13 +6186,13 @@
         <v>235</v>
       </c>
       <c r="B228" t="s">
-        <v>470</v>
+        <v>466</v>
       </c>
       <c r="C228" t="s">
-        <v>402</v>
+        <v>400</v>
       </c>
       <c r="H228" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
     </row>
     <row r="229" spans="1:8">
@@ -6206,13 +6200,13 @@
         <v>235</v>
       </c>
       <c r="B229" t="s">
-        <v>471</v>
+        <v>467</v>
       </c>
       <c r="C229" t="s">
-        <v>403</v>
+        <v>401</v>
       </c>
       <c r="H229" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
     </row>
     <row r="230" spans="1:8">
@@ -6220,13 +6214,13 @@
         <v>235</v>
       </c>
       <c r="B230" t="s">
-        <v>472</v>
+        <v>468</v>
       </c>
       <c r="C230" t="s">
-        <v>404</v>
+        <v>402</v>
       </c>
       <c r="H230" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
     </row>
     <row r="231" spans="1:8">
@@ -6234,10 +6228,10 @@
         <v>235</v>
       </c>
       <c r="B231" t="s">
-        <v>473</v>
+        <v>469</v>
       </c>
       <c r="C231" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="H231" t="s">
         <v>282</v>
@@ -6248,10 +6242,10 @@
         <v>235</v>
       </c>
       <c r="B232" t="s">
-        <v>474</v>
+        <v>470</v>
       </c>
       <c r="C232" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H232" t="s">
         <v>321</v>
@@ -6262,10 +6256,10 @@
         <v>235</v>
       </c>
       <c r="B233" t="s">
-        <v>475</v>
+        <v>471</v>
       </c>
       <c r="C233" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="H233" t="s">
         <v>334</v>
@@ -6276,10 +6270,10 @@
         <v>235</v>
       </c>
       <c r="B234" t="s">
-        <v>476</v>
+        <v>472</v>
       </c>
       <c r="C234" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="H234" t="s">
         <v>337</v>
@@ -6290,10 +6284,10 @@
         <v>235</v>
       </c>
       <c r="B235" t="s">
-        <v>477</v>
+        <v>473</v>
       </c>
       <c r="C235" t="s">
-        <v>406</v>
+        <v>404</v>
       </c>
       <c r="H235" t="s">
         <v>326</v>
@@ -6304,10 +6298,10 @@
         <v>235</v>
       </c>
       <c r="B236" t="s">
-        <v>478</v>
+        <v>474</v>
       </c>
       <c r="C236" t="s">
-        <v>408</v>
+        <v>406</v>
       </c>
       <c r="H236" t="s">
         <v>331</v>
@@ -6318,13 +6312,13 @@
         <v>235</v>
       </c>
       <c r="B237" t="s">
-        <v>479</v>
+        <v>475</v>
       </c>
       <c r="C237" t="s">
-        <v>409</v>
+        <v>407</v>
       </c>
       <c r="H237" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
     </row>
     <row r="238" spans="1:8">
@@ -6332,10 +6326,10 @@
         <v>235</v>
       </c>
       <c r="B238" t="s">
-        <v>480</v>
+        <v>476</v>
       </c>
       <c r="C238" t="s">
-        <v>410</v>
+        <v>408</v>
       </c>
       <c r="H238" t="s">
         <v>329</v>
@@ -6346,10 +6340,10 @@
         <v>235</v>
       </c>
       <c r="B239" t="s">
-        <v>481</v>
+        <v>477</v>
       </c>
       <c r="C239" t="s">
-        <v>411</v>
+        <v>409</v>
       </c>
       <c r="H239" t="s">
         <v>281</v>
@@ -6360,10 +6354,10 @@
         <v>235</v>
       </c>
       <c r="B240" t="s">
-        <v>482</v>
+        <v>478</v>
       </c>
       <c r="C240" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="H240" t="s">
         <v>287</v>
@@ -6374,10 +6368,10 @@
         <v>235</v>
       </c>
       <c r="B241" t="s">
-        <v>483</v>
+        <v>479</v>
       </c>
       <c r="C241" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="H241" t="s">
         <v>293</v>
@@ -6388,10 +6382,10 @@
         <v>235</v>
       </c>
       <c r="B242" t="s">
-        <v>484</v>
+        <v>480</v>
       </c>
       <c r="C242" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="H242" t="s">
         <v>292</v>
@@ -6402,10 +6396,10 @@
         <v>235</v>
       </c>
       <c r="B243" t="s">
-        <v>485</v>
+        <v>481</v>
       </c>
       <c r="C243" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="H243" t="s">
         <v>290</v>
@@ -6416,10 +6410,10 @@
         <v>235</v>
       </c>
       <c r="B244" t="s">
-        <v>414</v>
+        <v>412</v>
       </c>
       <c r="C244" t="s">
-        <v>415</v>
+        <v>413</v>
       </c>
       <c r="H244" t="s">
         <v>243</v>
@@ -6430,10 +6424,10 @@
         <v>235</v>
       </c>
       <c r="B245" t="s">
-        <v>416</v>
+        <v>414</v>
       </c>
       <c r="C245" t="s">
-        <v>397</v>
+        <v>395</v>
       </c>
       <c r="H245" t="s">
         <v>257</v>
@@ -6444,10 +6438,10 @@
         <v>235</v>
       </c>
       <c r="B246" t="s">
-        <v>486</v>
+        <v>482</v>
       </c>
       <c r="C246" t="s">
-        <v>373</v>
+        <v>371</v>
       </c>
       <c r="H246" t="s">
         <v>301</v>
@@ -6458,10 +6452,10 @@
         <v>235</v>
       </c>
       <c r="B247" t="s">
-        <v>487</v>
+        <v>483</v>
       </c>
       <c r="C247" t="s">
-        <v>417</v>
+        <v>415</v>
       </c>
       <c r="H247" t="s">
         <v>294</v>
@@ -6472,10 +6466,10 @@
         <v>235</v>
       </c>
       <c r="B248" t="s">
-        <v>488</v>
+        <v>484</v>
       </c>
       <c r="C248" t="s">
-        <v>418</v>
+        <v>416</v>
       </c>
       <c r="H248" t="s">
         <v>302</v>
@@ -6486,10 +6480,10 @@
         <v>235</v>
       </c>
       <c r="B249" t="s">
-        <v>489</v>
+        <v>485</v>
       </c>
       <c r="C249" t="s">
-        <v>412</v>
+        <v>410</v>
       </c>
       <c r="H249" t="s">
         <v>295</v>
@@ -6500,10 +6494,10 @@
         <v>235</v>
       </c>
       <c r="B250" t="s">
-        <v>419</v>
+        <v>417</v>
       </c>
       <c r="C250" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="H250" t="s">
         <v>260</v>
@@ -6514,10 +6508,10 @@
         <v>235</v>
       </c>
       <c r="B251" t="s">
-        <v>490</v>
+        <v>486</v>
       </c>
       <c r="C251" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="H251" t="s">
         <v>297</v>
@@ -6528,10 +6522,10 @@
         <v>235</v>
       </c>
       <c r="B252" t="s">
-        <v>491</v>
+        <v>487</v>
       </c>
       <c r="C252" t="s">
-        <v>420</v>
+        <v>418</v>
       </c>
       <c r="H252" t="s">
         <v>300</v>
@@ -6542,13 +6536,13 @@
         <v>235</v>
       </c>
       <c r="B253" t="s">
-        <v>492</v>
+        <v>488</v>
       </c>
       <c r="C253" t="s">
-        <v>407</v>
+        <v>405</v>
       </c>
       <c r="H253" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
     </row>
     <row r="254" spans="1:8">
@@ -6556,10 +6550,10 @@
         <v>235</v>
       </c>
       <c r="B254" t="s">
-        <v>493</v>
+        <v>489</v>
       </c>
       <c r="C254" t="s">
-        <v>421</v>
+        <v>419</v>
       </c>
       <c r="H254" t="s">
         <v>299</v>
@@ -6570,10 +6564,10 @@
         <v>235</v>
       </c>
       <c r="B255" t="s">
-        <v>494</v>
+        <v>490</v>
       </c>
       <c r="C255" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="H255" t="s">
         <v>328</v>
@@ -6584,13 +6578,13 @@
         <v>235</v>
       </c>
       <c r="B256" t="s">
-        <v>495</v>
+        <v>491</v>
       </c>
       <c r="C256" t="s">
-        <v>422</v>
+        <v>420</v>
       </c>
       <c r="H256" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
     </row>
     <row r="257" spans="1:8">
@@ -6598,10 +6592,10 @@
         <v>235</v>
       </c>
       <c r="B257" t="s">
-        <v>496</v>
+        <v>492</v>
       </c>
       <c r="C257" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="H257" t="s">
         <v>305</v>
@@ -6612,10 +6606,10 @@
         <v>235</v>
       </c>
       <c r="B258" t="s">
-        <v>423</v>
+        <v>421</v>
       </c>
       <c r="C258" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="H258" t="s">
         <v>245</v>
@@ -6626,10 +6620,10 @@
         <v>235</v>
       </c>
       <c r="B259" t="s">
-        <v>497</v>
+        <v>493</v>
       </c>
       <c r="C259" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="H259" t="s">
         <v>304</v>
@@ -6640,10 +6634,10 @@
         <v>235</v>
       </c>
       <c r="B260" t="s">
-        <v>498</v>
+        <v>494</v>
       </c>
       <c r="C260" t="s">
-        <v>425</v>
+        <v>423</v>
       </c>
       <c r="H260" t="s">
         <v>313</v>
@@ -6654,10 +6648,10 @@
         <v>235</v>
       </c>
       <c r="B261" t="s">
-        <v>499</v>
+        <v>495</v>
       </c>
       <c r="C261" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="H261" t="s">
         <v>307</v>
@@ -6668,10 +6662,10 @@
         <v>235</v>
       </c>
       <c r="B262" t="s">
-        <v>500</v>
+        <v>496</v>
       </c>
       <c r="C262" t="s">
-        <v>427</v>
+        <v>425</v>
       </c>
       <c r="H262" t="s">
         <v>303</v>
@@ -6682,13 +6676,13 @@
         <v>235</v>
       </c>
       <c r="B263" t="s">
-        <v>501</v>
+        <v>497</v>
       </c>
       <c r="C263" t="s">
-        <v>428</v>
+        <v>426</v>
       </c>
       <c r="H263" t="s">
-        <v>444</v>
+        <v>442</v>
       </c>
     </row>
     <row r="264" spans="1:8">
@@ -6696,10 +6690,10 @@
         <v>235</v>
       </c>
       <c r="B264" t="s">
-        <v>429</v>
+        <v>427</v>
       </c>
       <c r="C264" t="s">
-        <v>430</v>
+        <v>428</v>
       </c>
       <c r="H264" t="s">
         <v>268</v>
@@ -6710,10 +6704,10 @@
         <v>235</v>
       </c>
       <c r="B265" t="s">
-        <v>502</v>
+        <v>498</v>
       </c>
       <c r="C265" t="s">
-        <v>431</v>
+        <v>429</v>
       </c>
       <c r="H265" t="s">
         <v>309</v>
@@ -6724,10 +6718,10 @@
         <v>235</v>
       </c>
       <c r="B266" t="s">
-        <v>503</v>
+        <v>499</v>
       </c>
       <c r="C266" t="s">
-        <v>405</v>
+        <v>403</v>
       </c>
       <c r="H266" t="s">
         <v>306</v>
@@ -6738,10 +6732,10 @@
         <v>235</v>
       </c>
       <c r="B267" t="s">
-        <v>504</v>
+        <v>500</v>
       </c>
       <c r="C267" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="H267" t="s">
         <v>312</v>
@@ -6752,10 +6746,10 @@
         <v>235</v>
       </c>
       <c r="B268" t="s">
-        <v>505</v>
+        <v>501</v>
       </c>
       <c r="C268" t="s">
-        <v>432</v>
+        <v>430</v>
       </c>
       <c r="H268" t="s">
         <v>314</v>
@@ -6766,10 +6760,10 @@
         <v>235</v>
       </c>
       <c r="B269" t="s">
-        <v>433</v>
+        <v>431</v>
       </c>
       <c r="C269" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="H269" t="s">
         <v>271</v>
@@ -6780,10 +6774,10 @@
         <v>235</v>
       </c>
       <c r="B270" t="s">
-        <v>506</v>
+        <v>502</v>
       </c>
       <c r="C270" t="s">
-        <v>435</v>
+        <v>433</v>
       </c>
       <c r="H270" t="s">
         <v>315</v>
@@ -6794,10 +6788,10 @@
         <v>235</v>
       </c>
       <c r="B271" t="s">
-        <v>436</v>
+        <v>434</v>
       </c>
       <c r="C271" t="s">
-        <v>413</v>
+        <v>411</v>
       </c>
       <c r="H271" t="s">
         <v>264</v>
@@ -6808,10 +6802,10 @@
         <v>235</v>
       </c>
       <c r="B272" t="s">
-        <v>507</v>
+        <v>503</v>
       </c>
       <c r="C272" t="s">
-        <v>437</v>
+        <v>435</v>
       </c>
       <c r="H272" t="s">
         <v>296</v>
@@ -6822,10 +6816,10 @@
         <v>235</v>
       </c>
       <c r="B273" t="s">
-        <v>508</v>
+        <v>504</v>
       </c>
       <c r="C273" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="H273" t="s">
         <v>330</v>
@@ -6836,10 +6830,10 @@
         <v>235</v>
       </c>
       <c r="B274" t="s">
-        <v>509</v>
+        <v>505</v>
       </c>
       <c r="C274" t="s">
-        <v>438</v>
+        <v>436</v>
       </c>
       <c r="H274" t="s">
         <v>350</v>
@@ -6850,10 +6844,10 @@
         <v>235</v>
       </c>
       <c r="B275" t="s">
-        <v>510</v>
+        <v>506</v>
       </c>
       <c r="C275" t="s">
-        <v>439</v>
+        <v>437</v>
       </c>
       <c r="H275" t="s">
         <v>311</v>
@@ -6864,10 +6858,10 @@
         <v>235</v>
       </c>
       <c r="B276" t="s">
-        <v>511</v>
+        <v>507</v>
       </c>
       <c r="C276" t="s">
-        <v>440</v>
+        <v>438</v>
       </c>
       <c r="H276" t="s">
         <v>310</v>
@@ -6878,10 +6872,10 @@
         <v>235</v>
       </c>
       <c r="B277" t="s">
-        <v>441</v>
+        <v>439</v>
       </c>
       <c r="C277" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="H277" t="s">
         <v>269</v>
@@ -6892,10 +6886,10 @@
         <v>235</v>
       </c>
       <c r="B278" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="C278" t="s">
-        <v>442</v>
+        <v>440</v>
       </c>
       <c r="H278" t="s">
         <v>298</v>
@@ -6906,10 +6900,10 @@
         <v>235</v>
       </c>
       <c r="B279" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="C279" t="s">
-        <v>434</v>
+        <v>432</v>
       </c>
       <c r="H279" t="s">
         <v>291</v>
@@ -6920,10 +6914,10 @@
         <v>235</v>
       </c>
       <c r="B280" t="s">
-        <v>443</v>
+        <v>441</v>
       </c>
       <c r="C280" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="H280" t="s">
         <v>256</v>
@@ -6970,10 +6964,10 @@
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="22" t="s">
-        <v>445</v>
+        <v>510</v>
       </c>
       <c r="B2" s="23" t="s">
-        <v>446</v>
+        <v>511</v>
       </c>
       <c r="C2" s="21" t="s">
         <v>240</v>

</xml_diff>